<commit_message>
Updated test cases for authenticate, invalid errors and uncommented protect_json for testing
Updated test cases for authenticate, invalid errors and uncommented protect_json for testing
</commit_message>
<xml_diff>
--- a/metrics/bm.xlsx
+++ b/metrics/bm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\project-g6t6\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{259E50B4-9975-4B07-ADCE-9CE0FB716E2B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB4719FA-D77C-46EF-99C4-FD99AB009E83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1740" yWindow="2556" windowWidth="17280" windowHeight="10692" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="68">
   <si>
     <t>Severity</t>
   </si>
@@ -222,6 +222,18 @@
   </si>
   <si>
     <t>Unable to drop bid or drop section for the successful bid</t>
+  </si>
+  <si>
+    <t>json stop</t>
+  </si>
+  <si>
+    <t>Clearing logic not added in</t>
+  </si>
+  <si>
+    <t>authenticate</t>
+  </si>
+  <si>
+    <t>Case sensitivity for username not working for json, but working for manual</t>
   </si>
 </sst>
 </file>
@@ -1814,8 +1826,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2578,8 +2590,8 @@
         <v>5</v>
       </c>
       <c r="G19" s="40">
-        <f>SUM(F19:F22)</f>
-        <v>16</v>
+        <f>SUM(F19:F23)</f>
+        <v>21</v>
       </c>
       <c r="H19" s="14" t="str">
         <f>IF(G19&lt;10,Instructions!B7,Instructions!B8)</f>
@@ -2768,15 +2780,27 @@
       <c r="Z23" s="2"/>
     </row>
     <row r="24" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="26"/>
-      <c r="B24" s="17"/>
-      <c r="C24" s="21"/>
-      <c r="D24" s="14"/>
+      <c r="A24" s="26">
+        <v>22</v>
+      </c>
+      <c r="B24" s="17">
+        <v>4</v>
+      </c>
+      <c r="C24" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>65</v>
+      </c>
       <c r="E24" s="13" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
-      <c r="F24" s="13"/>
-      <c r="G24" s="35"/>
+      <c r="F24" s="13">
+        <v>1</v>
+      </c>
+      <c r="G24" s="40">
+        <v>2</v>
+      </c>
       <c r="H24" s="14"/>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
@@ -2798,15 +2822,25 @@
       <c r="Z24" s="2"/>
     </row>
     <row r="25" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="26"/>
-      <c r="B25" s="17"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="14"/>
+      <c r="A25" s="26">
+        <v>23</v>
+      </c>
+      <c r="B25" s="17">
+        <v>4</v>
+      </c>
+      <c r="C25" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>67</v>
+      </c>
       <c r="E25" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="F25" s="13"/>
-      <c r="G25" s="35"/>
+      <c r="F25" s="13">
+        <v>1</v>
+      </c>
+      <c r="G25" s="40"/>
       <c r="H25" s="14"/>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
@@ -30647,11 +30681,12 @@
       <c r="Z1000" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="G3:G6"/>
     <mergeCell ref="G7:G16"/>
     <mergeCell ref="G19:G23"/>
+    <mergeCell ref="G24:G25"/>
   </mergeCells>
   <conditionalFormatting sqref="H1:H1000">
     <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Stop current Development">
@@ -31753,19 +31788,19 @@
     <row r="24" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="34">
         <f>'Bug Metrics'!$A24</f>
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="B24" s="34">
         <f>'Bug Metrics'!$B24</f>
-        <v>0</v>
+        <v>4</v>
       </c>
-      <c r="C24" s="34">
+      <c r="C24" s="34" t="str">
         <f>'Bug Metrics'!$C24</f>
-        <v>0</v>
+        <v>json stop</v>
       </c>
-      <c r="D24" s="18">
+      <c r="D24" s="18" t="str">
         <f>'Bug Metrics'!$D24</f>
-        <v>0</v>
+        <v>Clearing logic not added in</v>
       </c>
       <c r="E24" s="31"/>
       <c r="F24" s="30"/>
@@ -31793,19 +31828,19 @@
     <row r="25" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="34">
         <f>'Bug Metrics'!$A25</f>
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B25" s="34">
         <f>'Bug Metrics'!$B25</f>
-        <v>0</v>
+        <v>4</v>
       </c>
-      <c r="C25" s="34">
+      <c r="C25" s="34" t="str">
         <f>'Bug Metrics'!$C25</f>
-        <v>0</v>
+        <v>authenticate</v>
       </c>
-      <c r="D25" s="18">
+      <c r="D25" s="18" t="str">
         <f>'Bug Metrics'!$D25</f>
-        <v>0</v>
+        <v>Case sensitivity for username not working for json, but working for manual</v>
       </c>
       <c r="E25" s="31"/>
       <c r="F25" s="30"/>

</xml_diff>